<commit_message>
Updated form for rest of fuels
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/egasoline/Model_Data_Base_egasoline.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/egasoline/Model_Data_Base_egasoline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/egasoline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="212" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2592EB2B-EF80-4362-A692-3AD1CC5F48ED}"/>
+  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB6F8CCB-99A6-4F6C-B671-2FF47C5DB0E8}"/>
   <bookViews>
-    <workbookView xWindow="-20940" yWindow="-20055" windowWidth="22710" windowHeight="17580" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-5745" yWindow="-18465" windowWidth="15240" windowHeight="12210" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="106">
   <si>
     <t>Unit</t>
   </si>
@@ -385,6 +385,12 @@
   </si>
   <si>
     <t>other_fuels</t>
+  </si>
+  <si>
+    <t>start_up_cost</t>
+  </si>
+  <si>
+    <t>shut_down_cost</t>
   </si>
 </sst>
 </file>
@@ -459,12 +465,6 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -474,6 +474,12 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -488,10 +494,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AE8" totalsRowShown="0">
-  <autoFilter ref="A1:AE8" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
-  <tableColumns count="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}" name="Table1" displayName="Table1" ref="A1:AG8" totalsRowShown="0">
+  <autoFilter ref="A1:AG8" xr:uid="{A55D93BB-3EF1-4249-80C0-A8E75E738393}"/>
+  <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{C73E51D0-1842-42F3-9C00-F0DBD2E661BE}" name="Unit"/>
     <tableColumn id="2" xr3:uid="{FA8BE796-DE15-407E-8998-92C973AE35A4}" name="Object_type"/>
     <tableColumn id="3" xr3:uid="{168877A6-E181-4446-9569-F36E8CEB8908}" name="Input1"/>
@@ -508,6 +518,8 @@
     <tableColumn id="33" xr3:uid="{D8C88D78-E68F-45EF-8A97-7C1F84821946}" name="start_up_Output2"/>
     <tableColumn id="9" xr3:uid="{50F936EF-D32C-4938-8FCA-291A6A3E82E6}" name="shut_down_Output1"/>
     <tableColumn id="20" xr3:uid="{84C680FD-12EA-4AE2-A238-57453A3D8C12}" name="shut_down_Output2"/>
+    <tableColumn id="18" xr3:uid="{B5D3C563-C4ED-480F-ACFC-F4264D03AF31}" name="start_up_cost"/>
+    <tableColumn id="17" xr3:uid="{95CFDBCB-0DEB-45F8-9B20-0EC6F791BEC7}" name="shut_down_cost"/>
     <tableColumn id="10" xr3:uid="{ACDE4024-BCA2-4145-B3BC-1A5A08F3EA7D}" name="Relation_In_In"/>
     <tableColumn id="11" xr3:uid="{8AEC88A1-B64A-43A2-AC89-3B27AB4ACAD7}" name="Relation_In_Out"/>
     <tableColumn id="25" xr3:uid="{95F69D80-80E7-42BD-B42F-59F3C3DC485B}" name="Relation_Out_Out"/>
@@ -521,8 +533,8 @@
     <tableColumn id="8" xr3:uid="{3D1E8A22-A849-4CDE-BBFA-E4A4C8F670B6}" name="minimum_op_point_Input2"/>
     <tableColumn id="12" xr3:uid="{2B7B5E32-3E86-4A68-A045-AA51A4A24280}" name="minimum_op_point_Output1"/>
     <tableColumn id="14" xr3:uid="{85E2E211-9879-417E-9645-71CD4680A1E8}" name="minimum_op_point_Output2"/>
-    <tableColumn id="15" xr3:uid="{752A45A3-76EA-4B92-8487-BB9B0C0F14F1}" name="resolution_output" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{0AB66AD0-7EF6-4EFA-A56D-DD0B84D8E912}" name="demand" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{752A45A3-76EA-4B92-8487-BB9B0C0F14F1}" name="resolution_output" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{0AB66AD0-7EF6-4EFA-A56D-DD0B84D8E912}" name="demand" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -537,7 +549,7 @@
     <tableColumn id="3" xr3:uid="{0B221EED-10BC-4C34-AC5E-37A826B1E8AE}" name="Input1"/>
     <tableColumn id="4" xr3:uid="{13095F0A-BCF6-40A3-B029-60B11214B154}" name="Input2"/>
     <tableColumn id="5" xr3:uid="{4C6B3E52-C4A2-4D67-B50B-9DAA089E0399}" name="Output1"/>
-    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Output2" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{551A8663-4680-4147-9E64-4B9A8EA76642}" name="Output2" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{5DF4D35D-AD4C-4648-BC90-B2BA8F975A09}" name="Connection_type"/>
     <tableColumn id="15" xr3:uid="{C0BCA9EF-0E20-40E5-9820-0EA6AB1DE457}" name="Cap_Input1_existing"/>
     <tableColumn id="14" xr3:uid="{D4F16D16-99DE-47DA-B08A-6DD56FEBC7A4}" name="Cap_Input1_max"/>
@@ -568,7 +580,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}" name="Table134" displayName="Table134" ref="A1:L5" totalsRowShown="0">
   <autoFilter ref="A1:L5" xr:uid="{070C7B69-9214-47B9-93F0-C6C6118ED7CC}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{59CF1CEF-E7FA-4B7F-9443-D4A6EAAB7A8F}" name="Storage" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{AEAA1B51-84C1-491F-81D5-7757B30BDCCD}" name="Object_type"/>
     <tableColumn id="6" xr3:uid="{FA5F8582-61FC-4A96-9E8D-E08E92F1962D}" name="value_before"/>
     <tableColumn id="5" xr3:uid="{58DBFD58-A0D2-4B31-B639-19B1628ABAC8}" name="value_start"/>
@@ -892,7 +904,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
-  <dimension ref="A1:AE8"/>
+  <dimension ref="A1:AG8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -910,16 +922,18 @@
     <col min="11" max="12" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -969,52 +983,58 @@
         <v>42</v>
       </c>
       <c r="Q1" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>47</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>29</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>33</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>89</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>90</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>91</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>92</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>48</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1024,17 +1044,17 @@
       <c r="E2" t="s">
         <v>80</v>
       </c>
-      <c r="R2">
-        <f t="shared" ref="R2:R8" si="0">1/0.795</f>
+      <c r="T2">
+        <f t="shared" ref="T2:T8" si="0">1/0.795</f>
         <v>1.2578616352201257</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>1.29</v>
       </c>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1056,29 +1076,29 @@
       <c r="G3">
         <v>0.75</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>5.8500000000000002E-3</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <f t="shared" si="0"/>
         <v>1.2578616352201257</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>1.76</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>4.34</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>0.02</v>
       </c>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1094,19 +1114,19 @@
       <c r="E4" t="s">
         <v>86</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>3.6010731197896975E-3</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>3.601073119789697E-3</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>26.81</v>
       </c>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1122,14 +1142,14 @@
       <c r="E5" t="s">
         <v>87</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <f t="shared" si="0"/>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1145,22 +1165,22 @@
       <c r="E6" t="s">
         <v>81</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>7.2437800000000002E-4</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>0.99</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>0.11929223744292237</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>1.4865951742627345E-3</v>
       </c>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1179,10 +1199,10 @@
       <c r="F7" t="s">
         <v>83</v>
       </c>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>75</v>
       </c>
@@ -1201,24 +1221,24 @@
       <c r="F8" t="s">
         <v>103</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>17.277901743828668</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <f t="shared" si="0"/>
         <v>1.2578616352201257</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AF8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="AG8" s="2">
         <v>20.192799999999998</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD6 AD8" xr:uid="{A4271B4C-6C14-4C97-BA49-1AE5EE50903D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2:AF6 AF8" xr:uid="{A4271B4C-6C14-4C97-BA49-1AE5EE50903D}">
       <formula1>"h, D, W, M, Q, Y"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>